<commit_message>
adding cores and prices to list, running large test
</commit_message>
<xml_diff>
--- a/doc/input_data.xlsx
+++ b/doc/input_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33660" windowHeight="19780" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -1620,11 +1620,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1179">
@@ -3141,8 +3141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3215,7 +3215,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1">
-        <v>5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="2" customFormat="1" ht="28">
@@ -3293,7 +3293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
@@ -3334,14 +3334,14 @@
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
       <c r="P1" s="8"/>
-      <c r="Q1" s="21" t="s">
+      <c r="Q1" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
     </row>
     <row r="2" spans="1:22" s="11" customFormat="1" ht="15">
       <c r="A2" s="11" t="s">
@@ -3553,7 +3553,7 @@
       <c r="B9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="21" t="s">
         <v>67</v>
       </c>
       <c r="D9" t="s">

</xml_diff>